<commit_message>
updated new doc on expen
</commit_message>
<xml_diff>
--- a/Daily report.xlsx
+++ b/Daily report.xlsx
@@ -8,15 +8,15 @@
   </bookViews>
   <sheets>
     <sheet name="Aman" sheetId="1" r:id="rId1"/>
-    <sheet name="sagar" sheetId="2" r:id="rId2"/>
-    <sheet name="shivang" sheetId="3" r:id="rId3"/>
+    <sheet name="shivang" sheetId="2" r:id="rId2"/>
+    <sheet name="sagar" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="86">
   <si>
     <t xml:space="preserve">Date </t>
   </si>
@@ -277,10 +277,27 @@
     <t>POST/CIENT FOLLOW UP</t>
   </si>
   <si>
-    <t>Two post ( NESTIN &amp; XPEN)  / MESSAGE TO EBNOY RWA FOLLOW UP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
+    <t xml:space="preserve">working on Bill Details,Generate Bill ,Active Bills ,deactive bills  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 am to 1pm ,2pm to still working on it </t>
+  </si>
+  <si>
+    <t>Employee table was missing in new database</t>
+  </si>
+  <si>
+    <t>pending</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Generates bills stil not working </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Two post ( NESTIN &amp; XPEN)  / MESSAGE TO EBNOY RWA FOLLOW UP/Research on SEO offline </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. 10 am - 12 30am
+2. 2am - 4 30pm
+3.4 30pm - 7 pm
 </t>
   </si>
 </sst>
@@ -664,8 +681,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -956,12 +973,14 @@
         <v>78</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="G11" s="9"/>
+        <v>85</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
@@ -976,15 +995,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.28515625" customWidth="1"/>
+    <col min="1" max="1" width="35.140625" customWidth="1"/>
     <col min="2" max="2" width="22.7109375" customWidth="1"/>
     <col min="3" max="3" width="24.5703125" customWidth="1"/>
     <col min="4" max="4" width="93" customWidth="1"/>
@@ -1187,6 +1206,9 @@
         <v>55</v>
       </c>
     </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="7"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1194,10 +1216,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1388,7 +1410,30 @@
       </c>
       <c r="E9" s="4"/>
       <c r="F9" s="4" t="s">
-        <v>55</v>
+        <v>81</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E10" t="s">
+        <v>80</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>